<commit_message>
Initial parameterisation of terpenoids model.
</commit_message>
<xml_diff>
--- a/models/terpenoids_kinetics.xlsx
+++ b/models/terpenoids_kinetics.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="24">
   <si>
     <t>kcat / s^-1</t>
   </si>
@@ -96,6 +96,9 @@
   <si>
     <t>geranyl diphosphate(3-)</t>
   </si>
+  <si>
+    <t>KEASLING</t>
+  </si>
 </sst>
 </file>
 
@@ -104,10 +107,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +146,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -153,103 +169,111 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="87">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="87">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -293,6 +317,8 @@
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -336,6 +362,8 @@
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,7 +696,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I17"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -729,23 +757,24 @@
       <c r="A3" s="1">
         <v>86497</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3">
         <v>4.8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>465</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <f>10^-3/60*$A$3*C3</f>
         <v>6.9197600000000001</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="3">
         <v>8.8300000000000003E-2</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="3">
         <v>0.01</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>0.6</v>
       </c>
       <c r="I3" s="2"/>
@@ -753,27 +782,27 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4">
+      <c r="B4" s="3">
         <v>1250</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>35</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <f>10^-3/60*$A$3*B4</f>
         <v>1802.0208333333335</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <f>10^-3/60*$A$3*C4</f>
         <v>50.456583333333334</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="3">
         <v>0.25</v>
       </c>
       <c r="I4" s="2"/>
@@ -781,20 +810,22 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5">
+      <c r="B5" s="3">
         <v>116</v>
       </c>
-      <c r="D5">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
         <f t="shared" ref="D5:D12" si="0">10^-3/60*$A$3*B5</f>
         <v>167.22753333333335</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
         <v>1.6E-2</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>0.02</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>0.08</v>
       </c>
       <c r="I5" s="2"/>
@@ -802,17 +833,20 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="D6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
         <f>3.8*11</f>
         <v>41.8</v>
       </c>
-      <c r="F6" s="2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="3">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="3">
         <v>1.06</v>
       </c>
       <c r="I6" s="2"/>
@@ -820,20 +854,22 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="B7">
+      <c r="B7" s="3">
         <v>296</v>
       </c>
-      <c r="D7">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>426.71853333333337</v>
       </c>
-      <c r="F7" s="2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
         <v>4.1999999999999996E-2</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>0.33</v>
       </c>
       <c r="I7" s="2"/>
@@ -841,20 +877,22 @@
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8">
+      <c r="B8" s="3">
         <v>216</v>
       </c>
-      <c r="D8">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>311.38920000000002</v>
       </c>
-      <c r="F8" s="2">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <v>2.4E-2</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>0.23</v>
       </c>
       <c r="I8" s="2"/>
@@ -862,20 +900,22 @@
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9">
+      <c r="B9" s="3">
         <v>1.8</v>
       </c>
-      <c r="D9">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>2.59491</v>
       </c>
-      <c r="F9" s="2">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>2.0999999999999998E-2</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>0.38</v>
       </c>
       <c r="I9" s="2"/>
@@ -883,17 +923,20 @@
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10">
+      <c r="B10" s="3">
         <v>12.6</v>
       </c>
-      <c r="D10">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>18.164370000000002</v>
       </c>
-      <c r="F10" s="2">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
         <v>0.05</v>
       </c>
-      <c r="H10" s="2">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
         <v>0.33</v>
       </c>
       <c r="I10" s="2"/>
@@ -901,17 +944,20 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="B11">
+      <c r="B11" s="3">
         <v>10.1</v>
       </c>
-      <c r="D11">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>14.560328333333334</v>
       </c>
-      <c r="F11" s="2">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="H11" s="2">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
         <v>0.27</v>
       </c>
       <c r="I11" s="2"/>
@@ -919,24 +965,34 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="B12">
+      <c r="B12" s="3">
         <v>63</v>
       </c>
-      <c r="D12">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>90.821850000000012</v>
       </c>
-      <c r="F12" s="2">
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
         <v>3.5000000000000001E-3</v>
       </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="F13" s="2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -945,31 +1001,25 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
-        <f>MEDIAN(B3:B13)</f>
-        <v>89.5</v>
-      </c>
-      <c r="C14" s="3">
-        <f>MEDIAN(C3:C13)</f>
-        <v>19.899999999999999</v>
-      </c>
-      <c r="D14" s="3">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="7">
         <f t="shared" ref="C14:H14" si="1">MEDIAN(D3:D13)</f>
         <v>129.02469166666668</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="7">
         <f t="shared" si="1"/>
         <v>28.688171666666666</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="7">
         <f t="shared" si="1"/>
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="7">
         <f t="shared" si="1"/>
         <v>0.33</v>
       </c>
@@ -978,16 +1028,10 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <f>AVERAGE(B3:B13)</f>
-        <v>245.68749999999997</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" ref="C15:H15" si="2">AVERAGE(C3:C13)</f>
-        <v>19.899999999999999</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C15:H15" si="2">AVERAGE(D3:D13)</f>
         <v>334.0297558333333</v>
       </c>
       <c r="E15" s="3">
@@ -1022,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82:D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1673,15 +1717,15 @@
       <c r="A82" t="s">
         <v>13</v>
       </c>
-      <c r="B82" s="3">
+      <c r="B82" s="7">
         <f>MEDIAN(B3:B81)</f>
         <v>2.3400000000000001E-2</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="7">
         <f t="shared" ref="C82:D82" si="0">MEDIAN(C3:C81)</f>
         <v>2.9500000000000004E-3</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="7">
         <f t="shared" si="0"/>
         <v>0.122</v>
       </c>
@@ -1716,10 +1760,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2129,31 +2173,31 @@
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
-      <c r="D15" s="3">
+      <c r="D15" s="7">
         <f t="shared" ref="C15:J15" si="2">MEDIAN(D3:D14)</f>
         <v>17.212903000000001</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="7">
         <f t="shared" si="2"/>
         <v>9.9414474985010912</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="7">
         <f t="shared" si="2"/>
         <v>0.40149999999999997</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="7">
         <f t="shared" ref="G15" si="3">MEDIAN(G3:G14)</f>
         <v>7.3000000000000009E-2</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="7">
         <f t="shared" ref="H15" si="4">MEDIAN(H3:H14)</f>
         <v>0.31</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="7">
         <f t="shared" ref="I15" si="5">MEDIAN(I3:I14)</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="7">
         <f t="shared" ref="J15" si="6">MEDIAN(J3:J14)</f>
         <v>0.17</v>
       </c>
@@ -2192,6 +2236,28 @@
         <f t="shared" si="7"/>
         <v>0.18733333333333335</v>
       </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2206,10 +2272,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D2"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2816,15 +2882,15 @@
       <c r="A67" t="s">
         <v>13</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B67" s="7">
         <f>MEDIAN(B3:B66)</f>
         <v>11.6</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="7">
         <f t="shared" ref="C67:D67" si="0">MEDIAN(C3:C66)</f>
         <v>0.1105</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="7">
         <f t="shared" si="0"/>
         <v>0.87985000000000002</v>
       </c>
@@ -2844,6 +2910,28 @@
       <c r="D68" s="3">
         <f t="shared" si="1"/>
         <v>1.2745</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="3">
+        <v>38</v>
+      </c>
+      <c r="C69" s="3">
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="3">
+        <v>6</v>
+      </c>
+      <c r="C70" s="3">
+        <v>4.1000000000000002E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2859,10 +2947,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B34" sqref="B34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3146,15 +3234,15 @@
       <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="7">
         <f>MEDIAN(B3:B33)</f>
         <v>10.199999999999999</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="7">
         <f t="shared" ref="C34:D34" si="0">MEDIAN(C3:C33)</f>
         <v>0.11</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="7">
         <f t="shared" si="0"/>
         <v>0.22900000000000001</v>
       </c>
@@ -3175,6 +3263,18 @@
         <f t="shared" si="1"/>
         <v>0.54552941176470593</v>
       </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="3">
+        <v>10</v>
+      </c>
+      <c r="C36" s="3">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="D36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3188,10 +3288,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F2"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68:F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3237,13 +3337,13 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1">
+      <c r="A3" s="6">
         <v>20508</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>2.1899999999999999E-2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <f>10^-3/60*$A$3*B3</f>
         <v>7.4854199999999996E-3</v>
       </c>
@@ -3870,19 +3970,19 @@
         <v>13</v>
       </c>
       <c r="B68" s="3"/>
-      <c r="C68" s="3">
+      <c r="C68" s="8">
         <f t="shared" ref="C68:F68" si="0">MEDIAN(C3:C67)</f>
         <v>7.4854199999999996E-3</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="7">
         <f t="shared" si="0"/>
         <v>0.69</v>
       </c>
-      <c r="E68" s="3">
+      <c r="E68" s="7">
         <f t="shared" si="0"/>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F68" s="3">
+      <c r="F68" s="7">
         <f t="shared" si="0"/>
         <v>1.2E-2</v>
       </c>
@@ -3892,7 +3992,7 @@
         <v>14</v>
       </c>
       <c r="B69" s="3"/>
-      <c r="C69" s="3">
+      <c r="C69" s="5">
         <f t="shared" ref="C69:F69" si="1">AVERAGE(C3:C67)</f>
         <v>7.4854199999999996E-3</v>
       </c>
@@ -3907,6 +4007,23 @@
       <c r="F69" s="3">
         <f t="shared" si="1"/>
         <v>0.26916261538461539</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="D70" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E70" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F70" s="3">
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3925,7 +4042,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3999,15 +4116,15 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="7">
         <f>MEDIAN(B3:B6)</f>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="7">
         <f t="shared" ref="C7:D7" si="0">MEDIAN(C3:C6)</f>
         <v>0.224</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="7">
         <f t="shared" si="0"/>
         <v>1.18E-2</v>
       </c>
@@ -4042,10 +4159,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4053,7 +4170,7 @@
     <col min="1" max="3" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3">
+    <row r="1" spans="1:3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -4061,7 +4178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:3">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -4069,7 +4186,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="1:3">
       <c r="B3" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
@@ -4077,31 +4194,49 @@
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="1:3">
       <c r="B4" s="3"/>
       <c r="C4" s="3">
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="1:3">
       <c r="B5" s="3"/>
       <c r="C5" s="3">
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="1:3">
       <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7">
+        <f>MEDIAN(B3:B6)</f>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C7" s="7">
+        <f>MEDIAN(C3:C6)</f>
+        <v>4.3E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <f>AVERAGE(B3:B6)</f>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C8" s="3">
+        <f>AVERAGE(C3:C6)</f>
+        <v>5.6124999999999994E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated kinetics factsheet for terpenoids.
</commit_message>
<xml_diff>
--- a/models/terpenoids_kinetics.xlsx
+++ b/models/terpenoids_kinetics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="25360" windowHeight="15220" tabRatio="742" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="742" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Q9FD70 2.3.1.9" sheetId="2" r:id="rId1"/>
@@ -1004,7 +1004,7 @@
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="7">
-        <f t="shared" ref="C14:H14" si="1">MEDIAN(D3:D13)</f>
+        <f t="shared" ref="D14:H14" si="1">MEDIAN(D3:D13)</f>
         <v>129.02469166666668</v>
       </c>
       <c r="E14" s="7">
@@ -1031,7 +1031,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <f t="shared" ref="C15:H15" si="2">AVERAGE(D3:D13)</f>
+        <f t="shared" ref="D15:H15" si="2">AVERAGE(D3:D13)</f>
         <v>334.0297558333333</v>
       </c>
       <c r="E15" s="3">
@@ -2174,7 +2174,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="7">
-        <f t="shared" ref="C15:J15" si="2">MEDIAN(D3:D14)</f>
+        <f t="shared" ref="D15:F15" si="2">MEDIAN(D3:D14)</f>
         <v>17.212903000000001</v>
       </c>
       <c r="E15" s="7">
@@ -2209,7 +2209,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3">
-        <f t="shared" ref="C16:J16" si="7">AVERAGE(D3:D14)</f>
+        <f t="shared" ref="D16:J16" si="7">AVERAGE(D3:D14)</f>
         <v>29.835858712962963</v>
       </c>
       <c r="E16" s="3">
@@ -3290,7 +3290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
       <selection activeCell="C68" sqref="C68:F68"/>
     </sheetView>
   </sheetViews>
@@ -4161,7 +4161,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated kinetic parameters / concentrations in the model.
</commit_message>
<xml_diff>
--- a/models/terpenoids_kinetics.xlsx
+++ b/models/terpenoids_kinetics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="742" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="742" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Q9FD70 2.3.1.9" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="28">
   <si>
     <t>kcat / s^-1</t>
   </si>
@@ -109,6 +109,9 @@
   <si>
     <t>(R)-5-diphosphonatomevalonate(4-)</t>
   </si>
+  <si>
+    <t>Ki / mM</t>
+  </si>
 </sst>
 </file>
 
@@ -184,8 +187,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="123">
+  <cellStyleXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,7 +333,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="123">
+  <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -384,6 +395,10 @@
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -445,6 +460,10 @@
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2420,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:G70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="G70" sqref="D68:G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2431,7 +2450,7 @@
     <col min="1" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6">
+    <row r="1" spans="2:7">
       <c r="B1" t="s">
         <v>24</v>
       </c>
@@ -2447,16 +2466,22 @@
       <c r="F1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="2:6">
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7">
       <c r="E2" t="s">
         <v>4</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7">
       <c r="B3" s="3">
         <v>-16.064087000000001</v>
       </c>
@@ -2473,8 +2498,11 @@
       <c r="F3" s="3">
         <v>2.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="2:6">
+      <c r="G3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
       <c r="D4" s="3">
         <v>4.3</v>
       </c>
@@ -2484,8 +2512,11 @@
       <c r="F4" s="3">
         <v>4.0300000000000002E-2</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="G4">
+        <v>2.3E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="D5" s="3">
         <v>5.2</v>
       </c>
@@ -2495,8 +2526,11 @@
       <c r="F5" s="3">
         <v>6.6000000000000003E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="G5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="D6" s="3">
         <v>8.6</v>
       </c>
@@ -2506,8 +2540,11 @@
       <c r="F6" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="G6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="D7" s="3">
         <v>10.5</v>
       </c>
@@ -2517,8 +2554,11 @@
       <c r="F7" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="G7">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
       <c r="D8" s="3">
         <v>12.7</v>
       </c>
@@ -2528,8 +2568,11 @@
       <c r="F8" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="G8">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="D9" s="3">
         <v>17.100000000000001</v>
       </c>
@@ -2539,8 +2582,11 @@
       <c r="F9" s="3">
         <v>9.1999999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="G9">
+        <v>0.11600000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
       <c r="D10" s="3">
         <v>21.9</v>
       </c>
@@ -2551,7 +2597,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:7">
       <c r="D11" s="3">
         <v>23.3</v>
       </c>
@@ -2562,7 +2608,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:7">
       <c r="D12" s="3">
         <v>28.5</v>
       </c>
@@ -2573,7 +2619,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:7">
       <c r="D13" s="3"/>
       <c r="E13" s="3">
         <v>7.4499999999999997E-2</v>
@@ -2582,7 +2628,7 @@
         <v>0.13100000000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:7">
       <c r="D14" s="3"/>
       <c r="E14" s="3">
         <v>7.5999999999999998E-2</v>
@@ -2591,7 +2637,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:7">
       <c r="D15" s="3"/>
       <c r="E15" s="3">
         <v>0.106</v>
@@ -2600,7 +2646,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:7">
       <c r="D16" s="3"/>
       <c r="E16" s="3">
         <v>0.111</v>
@@ -3025,21 +3071,21 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:7">
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3">
         <v>5.4</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:7">
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3">
         <v>7.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>13</v>
       </c>
@@ -3055,8 +3101,12 @@
         <f t="shared" si="0"/>
         <v>0.87985000000000002</v>
       </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="G67" s="6">
+        <f t="shared" ref="G67" si="1">MEDIAN(G3:G66)</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>14</v>
       </c>
@@ -3065,15 +3115,19 @@
         <v>13.52</v>
       </c>
       <c r="E68" s="3">
-        <f t="shared" ref="E68:F68" si="1">AVERAGE(E3:E66)</f>
+        <f t="shared" ref="E68:F68" si="2">AVERAGE(E3:E66)</f>
         <v>0.60165370370370375</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2745</v>
       </c>
-    </row>
-    <row r="69" spans="1:6">
+      <c r="G68" s="3">
+        <f t="shared" ref="G68" si="3">AVERAGE(G3:G66)</f>
+        <v>4.4757142857142863E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>23</v>
       </c>
@@ -3083,8 +3137,12 @@
       <c r="E69" s="3">
         <v>0.13100000000000001</v>
       </c>
-    </row>
-    <row r="70" spans="1:6">
+      <c r="F69" s="3"/>
+      <c r="G69" s="3">
+        <v>1.9E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -3093,6 +3151,10 @@
       </c>
       <c r="E70" s="3">
         <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3">
+        <v>4.5999999999999999E-3</v>
       </c>
     </row>
   </sheetData>
@@ -3110,8 +3172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:A36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3867,7 +3929,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E70" sqref="E70"/>
+      <selection activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4640,109 +4702,122 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+      <selection activeCell="B1" sqref="B1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="4" width="20.83203125" customWidth="1"/>
+    <col min="1" max="6" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="B2" t="s">
+    <row r="2" spans="1:6">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="B3" s="3">
+        <v>-13</v>
+      </c>
+      <c r="C3" s="3">
+        <f>EXP(-B3/4.184)/(0.008314*(273+37))</f>
+        <v>8.6738843334062299</v>
+      </c>
+      <c r="D3" s="3">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="E3" s="3">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="D3" s="3">
+      <c r="F3" s="3">
         <v>8.4000000000000003E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="B4" s="3">
+    <row r="4" spans="1:6">
+      <c r="D4" s="3">
         <v>1.4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="E4" s="3">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="D4" s="3">
+      <c r="F4" s="3">
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="3">
+    <row r="5" spans="1:6">
+      <c r="D5" s="3">
         <v>1.2E-2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="E5" s="3">
         <v>0.39</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
         <v>0.16300000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3">
+    <row r="6" spans="1:6">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>1.103</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
-        <f>MEDIAN(B3:B6)</f>
+      <c r="D7" s="6">
+        <f>MEDIAN(D3:D6)</f>
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C7" s="6">
-        <f t="shared" ref="C7:D7" si="0">MEDIAN(C3:C6)</f>
+      <c r="E7" s="6">
+        <f t="shared" ref="E7:F7" si="0">MEDIAN(E3:E6)</f>
         <v>0.224</v>
       </c>
-      <c r="D7" s="6">
+      <c r="F7" s="6">
         <f t="shared" si="0"/>
         <v>1.18E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3">
-        <f>AVERAGE(B3:B6)</f>
+      <c r="D8" s="3">
+        <f>AVERAGE(D3:D6)</f>
         <v>0.49899999999999994</v>
       </c>
-      <c r="C8" s="3">
-        <f t="shared" ref="C8:D8" si="1">AVERAGE(C3:C6)</f>
+      <c r="E8" s="3">
+        <f t="shared" ref="E8:F8" si="1">AVERAGE(E3:E6)</f>
         <v>0.39065</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>5.854666666666667E-2</v>
       </c>
@@ -4760,87 +4835,101 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="3" width="20.83203125" customWidth="1"/>
+    <col min="1" max="5" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="B2" t="s">
+    <row r="2" spans="1:5">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="B3" s="3">
+        <v>-28.049987999999999</v>
+      </c>
+      <c r="C3" s="3">
+        <f>EXP(-B3/4.184)/(0.008314*(273+37))</f>
+        <v>316.50852335880228</v>
+      </c>
+      <c r="D3" s="3">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="E3" s="3">
         <v>1.25E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
+    <row r="4" spans="1:5">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3">
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
+    <row r="5" spans="1:5">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3">
+    <row r="6" spans="1:5">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>1.26E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6">
-        <f>MEDIAN(B3:B6)</f>
+      <c r="D7" s="6">
+        <f>MEDIAN(D3:D6)</f>
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="C7" s="6">
-        <f>MEDIAN(C3:C6)</f>
+      <c r="E7" s="6">
+        <f>MEDIAN(E3:E6)</f>
         <v>4.3E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3">
-        <f>AVERAGE(B3:B6)</f>
+      <c r="D8" s="3">
+        <f>AVERAGE(D3:D6)</f>
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="C8" s="3">
-        <f>AVERAGE(C3:C6)</f>
+      <c r="E8" s="3">
+        <f>AVERAGE(E3:E6)</f>
         <v>5.6124999999999994E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Updated terpenoids kinetic parameters factsheet.
</commit_message>
<xml_diff>
--- a/models/terpenoids_kinetics.xlsx
+++ b/models/terpenoids_kinetics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="742" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="742"/>
   </bookViews>
   <sheets>
     <sheet name="Q9FD70 2.3.1.9" sheetId="2" r:id="rId1"/>
@@ -117,8 +117,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -187,7 +188,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -319,8 +320,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -332,8 +335,9 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="133">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -399,6 +403,7 @@
     <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -464,6 +469,7 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -795,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -929,7 +935,10 @@
     </row>
     <row r="5" spans="1:13">
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="C5" s="11">
+        <f>ABS(C3-C4)/C3</f>
+        <v>27.306715677867441</v>
+      </c>
       <c r="D5" s="3">
         <v>116</v>
       </c>
@@ -1914,7 +1923,7 @@
   <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2073,6 +2082,10 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17">
+      <c r="C5" s="11">
+        <f>ABS(C3-C4)/C3</f>
+        <v>0.60620707645607819</v>
+      </c>
       <c r="D5" s="3">
         <v>1.2030000000000001</v>
       </c>
@@ -3172,7 +3185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3929,7 +3942,7 @@
   <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4054,6 +4067,10 @@
       </c>
     </row>
     <row r="7" spans="1:8">
+      <c r="C7" s="11">
+        <f>ABS(C3-C4)/C3</f>
+        <v>0.9831436373793907</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3">

</xml_diff>